<commit_message>
Automação da tabela de análise
</commit_message>
<xml_diff>
--- a/Arquivos/Resultados/Heurísticas.xlsx
+++ b/Arquivos/Resultados/Heurísticas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="K = n|4" sheetId="1" r:id="rId1"/>
@@ -305,10 +305,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -325,7 +325,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,28 +398,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -369,7 +408,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -385,14 +424,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -417,45 +456,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -520,6 +520,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -538,6 +544,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -550,7 +580,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,7 +646,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,7 +670,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,121 +700,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,8 +859,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -880,50 +895,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -943,161 +930,174 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1526,8 +1526,8 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA30" sqref="AA30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -4400,8 +4400,8 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AC25" sqref="AC25:AD26"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -7279,8 +7279,8 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z29" sqref="Z29"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Atualizando tabelas de resultados
</commit_message>
<xml_diff>
--- a/Arquivos/Resultados/Heurísticas.xlsx
+++ b/Arquivos/Resultados/Heurísticas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500"/>
+    <workbookView windowWidth="13725" windowHeight="12870" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="K = n|4" sheetId="1" r:id="rId1"/>
@@ -305,8 +305,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -325,28 +325,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -361,7 +347,90 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,6 +439,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -385,91 +461,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -520,7 +520,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,7 +556,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,25 +580,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +598,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,7 +622,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,31 +634,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,37 +676,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,7 +694,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,11 +856,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -880,17 +886,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -900,17 +902,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -949,6 +940,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -956,148 +956,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1526,8 +1526,8 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AA30" sqref="AA30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -4400,8 +4400,8 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3:AA26"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -7279,8 +7279,8 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3:AA26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y25" sqref="Y25:Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>

</xml_diff>